<commit_message>
pta_sim_board_app: initial sent to user test version
- basic working
</commit_message>
<xml_diff>
--- a/embeded/pta_sim_board_app/DOC/pin分配.xlsx
+++ b/embeded/pta_sim_board_app/DOC/pin分配.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE357BBC-15F3-4252-93D1-FF74934FF7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19395" windowHeight="11475"/>
   </bookViews>
   <sheets>
     <sheet name="PTA_SIM板v1.0" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">PTA_SIM板v1.0!$A$1:$D$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PTA_SIM板v1.0!$A$1:$D$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve"> 序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -68,47 +67,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PB10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PB11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GREEN LED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TXD串口发uart3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RXD串口收uart3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AO</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AI</t>
+    <t>PA4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUTPUT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,7 +137,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -171,9 +146,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -193,7 +165,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -235,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,27 +239,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,24 +273,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -512,14 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.1328125" style="2" customWidth="1"/>
     <col min="2" max="3" width="13.73046875" style="2" customWidth="1"/>
@@ -529,7 +465,7 @@
     <col min="7" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -549,109 +485,53 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>